<commit_message>
Se realiza las pruebas de estres SVM
</commit_message>
<xml_diff>
--- a/pruebas-funcionales/seguro-para-viaje/pruebas-funcionales.xlsx
+++ b/pruebas-funcionales/seguro-para-viaje/pruebas-funcionales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\OneDrive\Documentos\Cristian\Prueba-tecnica\prueba-tecnica\pruebas-funcionales\seguro-para-viaje\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8947F4-50DC-4C4D-80D2-608A6113A86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F08097-D8AB-46CA-8F89-70878C36C837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PF-1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Parametrización" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -613,20 +612,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -652,9 +654,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -667,17 +666,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -917,18 +916,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -948,16 +947,16 @@
       <c r="AA1" s="5"/>
     </row>
     <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -977,16 +976,16 @@
       <c r="AA2" s="5"/>
     </row>
     <row r="3" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1016,24 +1015,24 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="19" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -1121,19 +1120,19 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
@@ -1163,15 +1162,15 @@
         <v>22</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>32</v>
       </c>
       <c r="I8" s="15"/>
@@ -1204,15 +1203,15 @@
         <v>23</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>32</v>
       </c>
       <c r="I9" s="15"/>
@@ -1245,15 +1244,15 @@
         <v>24</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>32</v>
       </c>
       <c r="I10" s="15"/>
@@ -1286,15 +1285,15 @@
         <v>25</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>30</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="15"/>
@@ -1323,15 +1322,15 @@
       <c r="A12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1354,17 +1353,17 @@
       <c r="A13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1390,13 +1389,13 @@
       <c r="B14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="15"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -29229,14 +29228,12 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="A12:J12"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="B14:J14"/>
@@ -29253,14 +29250,16 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="A12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29295,42 +29294,42 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -29343,24 +29342,24 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="19" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
@@ -29397,19 +29396,19 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
@@ -29422,15 +29421,15 @@
         <v>34</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="15"/>
@@ -29446,15 +29445,15 @@
         <v>35</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>43</v>
       </c>
       <c r="I9" s="15"/>
@@ -29470,15 +29469,15 @@
         <v>41</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>47</v>
       </c>
       <c r="I10" s="15"/>
@@ -29494,15 +29493,15 @@
         <v>44</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>49</v>
       </c>
       <c r="I11" s="15"/>
@@ -29518,15 +29517,15 @@
         <v>36</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="17" t="s">
         <v>52</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>53</v>
       </c>
       <c r="I12" s="15"/>
@@ -29542,15 +29541,15 @@
         <v>54</v>
       </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>55</v>
       </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>56</v>
       </c>
       <c r="G13" s="15"/>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="16" t="s">
         <v>57</v>
       </c>
       <c r="I13" s="15"/>
@@ -29566,15 +29565,15 @@
         <v>34</v>
       </c>
       <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>38</v>
       </c>
       <c r="G14" s="15"/>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="16" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="15"/>
@@ -29586,31 +29585,31 @@
       <c r="A15" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
@@ -29619,13 +29618,13 @@
       <c r="B17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -29635,13 +29634,13 @@
       <c r="B18" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -29651,13 +29650,13 @@
       <c r="B19" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -29667,24 +29666,46 @@
       <c r="B20" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
@@ -29693,38 +29714,16 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29759,42 +29758,42 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -29807,24 +29806,24 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="19" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
@@ -29861,19 +29860,19 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
@@ -29886,15 +29885,15 @@
         <v>61</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>63</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>64</v>
       </c>
       <c r="I8" s="15"/>
@@ -29910,15 +29909,15 @@
         <v>34</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>65</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>67</v>
       </c>
       <c r="I9" s="15"/>
@@ -29934,15 +29933,15 @@
         <v>62</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>70</v>
       </c>
       <c r="I10" s="15"/>
@@ -29958,15 +29957,15 @@
         <v>61</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>63</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>64</v>
       </c>
       <c r="I11" s="15"/>
@@ -29982,15 +29981,15 @@
         <v>34</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="17" t="s">
         <v>65</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>66</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>67</v>
       </c>
       <c r="I12" s="15"/>
@@ -30002,31 +30001,31 @@
       <c r="A13" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
@@ -30035,17 +30034,38 @@
       <c r="B15" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -30061,27 +30081,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -30116,42 +30115,42 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -30164,24 +30163,24 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="19" t="s">
         <v>85</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
@@ -30218,19 +30217,19 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
@@ -30243,15 +30242,15 @@
         <v>61</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>63</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>64</v>
       </c>
       <c r="I8" s="15"/>
@@ -30267,15 +30266,15 @@
         <v>34</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>76</v>
       </c>
       <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>77</v>
       </c>
       <c r="G9" s="15"/>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>78</v>
       </c>
       <c r="I9" s="15"/>
@@ -30291,15 +30290,15 @@
         <v>72</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>70</v>
       </c>
       <c r="I10" s="15"/>
@@ -30313,18 +30312,18 @@
         <v>79</v>
       </c>
       <c r="C11" s="38"/>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="17" t="s">
+      <c r="E11" s="21"/>
+      <c r="F11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="17" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="37"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="10" t="s">
         <v>12</v>
       </c>
@@ -30337,18 +30336,18 @@
         <v>73</v>
       </c>
       <c r="C12" s="38"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="17" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="17" t="s">
+      <c r="G12" s="21"/>
+      <c r="H12" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="37"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="10" t="s">
         <v>12</v>
       </c>
@@ -30361,18 +30360,18 @@
         <v>74</v>
       </c>
       <c r="C13" s="38"/>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="21"/>
+      <c r="F13" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="17" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="37"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="10" t="s">
         <v>12</v>
       </c>
@@ -30385,18 +30384,18 @@
         <v>75</v>
       </c>
       <c r="C14" s="38"/>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="21"/>
+      <c r="F14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="17" t="s">
+      <c r="G14" s="21"/>
+      <c r="H14" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="I14" s="37"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="10" t="s">
         <v>12</v>
       </c>
@@ -30409,15 +30408,15 @@
         <v>61</v>
       </c>
       <c r="C15" s="15"/>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="17" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="16" t="s">
         <v>64</v>
       </c>
       <c r="I15" s="15"/>
@@ -30433,15 +30432,15 @@
         <v>34</v>
       </c>
       <c r="C16" s="15"/>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>76</v>
       </c>
       <c r="E16" s="15"/>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>77</v>
       </c>
       <c r="G16" s="15"/>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="16" t="s">
         <v>78</v>
       </c>
       <c r="I16" s="15"/>
@@ -30453,31 +30452,31 @@
       <c r="A17" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
@@ -30486,22 +30485,48 @@
       <c r="B19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
       <c r="J19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="B19:J19"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
@@ -30518,37 +30543,11 @@
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="A17:J17"/>
     <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -30577,48 +30576,48 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="37"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -30631,24 +30630,24 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="19" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
@@ -30685,24 +30684,24 @@
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="34" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -30710,15 +30709,15 @@
         <v>94</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>95</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>96</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>97</v>
       </c>
       <c r="I8" s="15"/>
@@ -30742,21 +30741,21 @@
     </row>
     <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>98</v>
       </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>100</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>101</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>101</v>
       </c>
       <c r="I10" s="15"/>
@@ -30780,21 +30779,21 @@
     </row>
     <row r="12" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>103</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="17" t="s">
         <v>104</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>101</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>101</v>
       </c>
       <c r="I12" s="15"/>
@@ -30806,66 +30805,81 @@
       <c r="A13" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A13:J13"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="B7:C7"/>
@@ -30882,21 +30896,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>